<commit_message>
Historia de usuario HU-09
Adición de historia de usuario al proyecto IMC, con la funcionalidad de registro como usuario administrador del programa
</commit_message>
<xml_diff>
--- a/Historias_UsuarioIMC_EQ8_GRUPO19_resumen.xlsx
+++ b/Historias_UsuarioIMC_EQ8_GRUPO19_resumen.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DOCUMENTOS JESSI\MISION TIC 2022\CICLO 3\DESARROLLO IMC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{882B382C-7A64-4CBC-A375-147BCD65054B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A32D281-FACD-45E6-965B-8FCB65A660B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen HU" sheetId="1" r:id="rId1"/>
@@ -22,13 +22,14 @@
     <sheet name="HU06" sheetId="15" r:id="rId7"/>
     <sheet name="HU07" sheetId="16" r:id="rId8"/>
     <sheet name="HU08" sheetId="17" r:id="rId9"/>
+    <sheet name="HU09" sheetId="18" r:id="rId10"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="56">
   <si>
     <t>Rol</t>
   </si>
@@ -218,6 +219,24 @@
   </si>
   <si>
     <t>HU08</t>
+  </si>
+  <si>
+    <t>HU09</t>
+  </si>
+  <si>
+    <t>HU-09</t>
+  </si>
+  <si>
+    <t>Necesito registrarme para acceder al contenido del programa</t>
+  </si>
+  <si>
+    <t>El administrador de la aplicación será  el nutricionista o médico tratante, quien debe registrarse en el programa para acceder a todo el contenido y llevar el control de sus pacientes.</t>
+  </si>
+  <si>
+    <t>En la pantalla de inicio se encontrará un botón para acceso al sistema IMC, al dar clic en el botón se abre una nueva ventana que solicita la infomación de  usuarios registrados como:
+1. Correo electrónico del médico tratante
+2.  Contraseña de acceso al sistema.
+Para el caso de usuarios administradores que no se encuentran registrados aparecerá un botón denominado "Registrarse" al dar clic en ese bot ón se habilitará un formulario para diligenciar la información personal y profesional.</t>
   </si>
 </sst>
 </file>
@@ -768,14 +787,74 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:srcRect l="21935" t="24345" r="21318" b="10825"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="email">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="552450" y="419099"/>
           <a:ext cx="6934199" cy="4453853"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>666882</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Imagen 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28C88594-937D-4DB9-9CB8-0AFE980F427F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="email">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="685800" y="266699"/>
+          <a:ext cx="5315082" cy="3352801"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -987,8 +1066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y1006"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView topLeftCell="A12" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1294,12 +1373,25 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
+    <row r="14" spans="1:25" ht="186.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="15" spans="1:25" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="1"/>
@@ -8259,6 +8351,7 @@
     <hyperlink ref="G11" location="'HU06'!A1" display="HU06" xr:uid="{98D2ACE9-85D9-4255-A989-BF9A5F875FFA}"/>
     <hyperlink ref="G12" location="'HU07'!A1" display="HU07" xr:uid="{1247B1AF-AA59-43E5-B03D-411C687B924C}"/>
     <hyperlink ref="G13" location="'HU08'!A1" display="HU08" xr:uid="{EE6CED8D-5362-4DAB-84B7-54915273683B}"/>
+    <hyperlink ref="G14" location="'HU09'!A1" display="HU09" xr:uid="{C0E0F837-C815-4F10-9B7A-45294E3F74C5}"/>
   </hyperlinks>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8266,6 +8359,21 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F42C9B7-8A0D-4862-AB6E-552D639D062E}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -8377,7 +8485,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>